<commit_message>
Updated Test Cases for ORder
</commit_message>
<xml_diff>
--- a/documentation/quality/Test Documents/05 TC - Orders.xlsx
+++ b/documentation/quality/Test Documents/05 TC - Orders.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\HostedRBI\apc-softdev-it111-06\documentation\quality\Test Documents\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="-135" windowWidth="19350" windowHeight="8010"/>
   </bookViews>
@@ -11,7 +16,7 @@
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
@@ -1363,11 +1368,11 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd;@"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1722,6 +1727,18 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1"/>
@@ -1734,86 +1751,11 @@
     <xf numFmtId="10" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="12">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF7030A0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF7030A0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF7030A0"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="3">
     <dxf>
       <fill>
         <patternFill>
@@ -1840,6 +1782,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -1888,7 +1833,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1920,9 +1865,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1954,6 +1900,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -2129,14 +2076,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O309"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:G1"/>
+      <selection activeCell="L3" sqref="L3:L4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12.5703125" customWidth="1"/>
     <col min="2" max="2" width="21.7109375" bestFit="1" customWidth="1"/>
@@ -2146,27 +2093,27 @@
     <col min="6" max="6" width="9.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15">
-      <c r="A1" s="56" t="s">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A1" s="60" t="s">
         <v>41</v>
       </c>
-      <c r="B1" s="57"/>
-      <c r="C1" s="57"/>
-      <c r="D1" s="57"/>
-      <c r="E1" s="57"/>
-      <c r="F1" s="57"/>
-      <c r="G1" s="58"/>
-    </row>
-    <row r="2" spans="1:15">
-      <c r="A2" s="53" t="s">
+      <c r="B1" s="61"/>
+      <c r="C1" s="61"/>
+      <c r="D1" s="61"/>
+      <c r="E1" s="61"/>
+      <c r="F1" s="61"/>
+      <c r="G1" s="62"/>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A2" s="57" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="54"/>
-      <c r="C2" s="54"/>
-      <c r="D2" s="54"/>
-      <c r="E2" s="54"/>
-      <c r="F2" s="54"/>
-      <c r="G2" s="55"/>
+      <c r="B2" s="58"/>
+      <c r="C2" s="58"/>
+      <c r="D2" s="58"/>
+      <c r="E2" s="58"/>
+      <c r="F2" s="58"/>
+      <c r="G2" s="59"/>
       <c r="I2" s="43" t="s">
         <v>143</v>
       </c>
@@ -2183,54 +2130,54 @@
         <v>146</v>
       </c>
     </row>
-    <row r="3" spans="1:15">
-      <c r="A3" s="53" t="s">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A3" s="57" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="54"/>
-      <c r="C3" s="54"/>
-      <c r="D3" s="54"/>
-      <c r="E3" s="54"/>
-      <c r="F3" s="54"/>
-      <c r="G3" s="55"/>
-      <c r="I3" s="59">
-        <f>AVERAGE(Sheet2!B17/64)</f>
+      <c r="B3" s="58"/>
+      <c r="C3" s="58"/>
+      <c r="D3" s="58"/>
+      <c r="E3" s="58"/>
+      <c r="F3" s="58"/>
+      <c r="G3" s="59"/>
+      <c r="I3" s="63">
+        <f>AVERAGE(Sheet2!B18/74)</f>
         <v>0</v>
       </c>
-      <c r="J3" s="59">
-        <f>AVERAGE(Sheet2!C17/64)</f>
+      <c r="J3" s="63">
+        <f>AVERAGE(Sheet2!C18/74)</f>
         <v>0</v>
       </c>
-      <c r="K3" s="59">
-        <f>AVERAGE(Sheet2!D17/64)</f>
-        <v>0.984375</v>
-      </c>
-      <c r="L3" s="59">
-        <f>AVERAGE(Sheet2!E17/64)</f>
+      <c r="K3" s="63">
+        <f>AVERAGE(Sheet2!D18/74)</f>
+        <v>1</v>
+      </c>
+      <c r="L3" s="63">
+        <f>AVERAGE(Sheet2!E18/74)</f>
         <v>0</v>
       </c>
-      <c r="M3" s="59">
+      <c r="M3" s="63">
         <f>SUM(I3:L4)</f>
-        <v>0.984375</v>
-      </c>
-    </row>
-    <row r="4" spans="1:15" ht="15.75" thickBot="1">
-      <c r="A4" s="50" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="54" t="s">
         <v>40</v>
       </c>
-      <c r="B4" s="51"/>
-      <c r="C4" s="51"/>
-      <c r="D4" s="51"/>
-      <c r="E4" s="51"/>
-      <c r="F4" s="51"/>
-      <c r="G4" s="52"/>
-      <c r="I4" s="59"/>
-      <c r="J4" s="59"/>
-      <c r="K4" s="59"/>
-      <c r="L4" s="59"/>
-      <c r="M4" s="59"/>
-    </row>
-    <row r="5" spans="1:15">
+      <c r="B4" s="55"/>
+      <c r="C4" s="55"/>
+      <c r="D4" s="55"/>
+      <c r="E4" s="55"/>
+      <c r="F4" s="55"/>
+      <c r="G4" s="56"/>
+      <c r="I4" s="63"/>
+      <c r="J4" s="63"/>
+      <c r="K4" s="63"/>
+      <c r="L4" s="63"/>
+      <c r="M4" s="63"/>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5" s="18">
         <v>5</v>
       </c>
@@ -2243,7 +2190,7 @@
       <c r="F5" s="20"/>
       <c r="G5" s="21"/>
     </row>
-    <row r="6" spans="1:15">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6" s="22" t="s">
         <v>2</v>
       </c>
@@ -2266,7 +2213,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:15" ht="60.75" customHeight="1" thickBot="1">
+    <row r="7" spans="1:15" ht="60.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="24" t="s">
         <v>42</v>
       </c>
@@ -2282,15 +2229,15 @@
         <v>7</v>
       </c>
       <c r="G7" s="25"/>
-      <c r="I7" s="63"/>
-      <c r="J7" s="63"/>
-      <c r="K7" s="63"/>
-      <c r="L7" s="63"/>
-      <c r="M7" s="63"/>
-      <c r="N7" s="63"/>
-      <c r="O7" s="63"/>
-    </row>
-    <row r="8" spans="1:15" ht="150.75" thickBot="1">
+      <c r="I7" s="50"/>
+      <c r="J7" s="50"/>
+      <c r="K7" s="50"/>
+      <c r="L7" s="50"/>
+      <c r="M7" s="50"/>
+      <c r="N7" s="50"/>
+      <c r="O7" s="50"/>
+    </row>
+    <row r="8" spans="1:15" ht="150.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="24" t="s">
         <v>43</v>
       </c>
@@ -2306,17 +2253,17 @@
         <v>7</v>
       </c>
       <c r="G8" s="25"/>
-      <c r="I8" s="60" t="s">
+      <c r="I8" s="51" t="s">
         <v>244</v>
       </c>
-      <c r="J8" s="61"/>
-      <c r="K8" s="61"/>
-      <c r="L8" s="61"/>
-      <c r="M8" s="61"/>
-      <c r="N8" s="61"/>
-      <c r="O8" s="62"/>
-    </row>
-    <row r="9" spans="1:15" ht="135">
+      <c r="J8" s="52"/>
+      <c r="K8" s="52"/>
+      <c r="L8" s="52"/>
+      <c r="M8" s="52"/>
+      <c r="N8" s="52"/>
+      <c r="O8" s="53"/>
+    </row>
+    <row r="9" spans="1:15" ht="135" x14ac:dyDescent="0.25">
       <c r="A9" s="24" t="s">
         <v>44</v>
       </c>
@@ -2333,7 +2280,7 @@
       </c>
       <c r="G9" s="25"/>
     </row>
-    <row r="10" spans="1:15" ht="210">
+    <row r="10" spans="1:15" ht="210" x14ac:dyDescent="0.25">
       <c r="A10" s="24" t="s">
         <v>45</v>
       </c>
@@ -2350,7 +2297,7 @@
       </c>
       <c r="G10" s="25"/>
     </row>
-    <row r="11" spans="1:15" ht="135">
+    <row r="11" spans="1:15" ht="135" x14ac:dyDescent="0.25">
       <c r="A11" s="24" t="s">
         <v>46</v>
       </c>
@@ -2367,7 +2314,7 @@
       </c>
       <c r="G11" s="25"/>
     </row>
-    <row r="12" spans="1:15" s="12" customFormat="1">
+    <row r="12" spans="1:15" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="26">
         <v>5.0999999999999996</v>
       </c>
@@ -2380,7 +2327,7 @@
       <c r="F12" s="3"/>
       <c r="G12" s="27"/>
     </row>
-    <row r="13" spans="1:15" ht="45">
+    <row r="13" spans="1:15" ht="45" x14ac:dyDescent="0.25">
       <c r="A13" s="24" t="s">
         <v>51</v>
       </c>
@@ -2397,7 +2344,7 @@
       </c>
       <c r="G13" s="25"/>
     </row>
-    <row r="14" spans="1:15" ht="60">
+    <row r="14" spans="1:15" ht="60" x14ac:dyDescent="0.25">
       <c r="A14" s="24" t="s">
         <v>52</v>
       </c>
@@ -2414,7 +2361,7 @@
       </c>
       <c r="G14" s="25"/>
     </row>
-    <row r="15" spans="1:15" ht="45">
+    <row r="15" spans="1:15" ht="45" x14ac:dyDescent="0.25">
       <c r="A15" s="24" t="s">
         <v>53</v>
       </c>
@@ -2431,7 +2378,7 @@
       </c>
       <c r="G15" s="25"/>
     </row>
-    <row r="16" spans="1:15" ht="30">
+    <row r="16" spans="1:15" ht="30" x14ac:dyDescent="0.25">
       <c r="A16" s="28">
         <v>5.2</v>
       </c>
@@ -2444,7 +2391,7 @@
       <c r="F16" s="8"/>
       <c r="G16" s="29"/>
     </row>
-    <row r="17" spans="1:7" ht="60">
+    <row r="17" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A17" s="24" t="s">
         <v>56</v>
       </c>
@@ -2461,7 +2408,7 @@
       </c>
       <c r="G17" s="25"/>
     </row>
-    <row r="18" spans="1:7" ht="120">
+    <row r="18" spans="1:7" ht="120" x14ac:dyDescent="0.25">
       <c r="A18" s="24" t="s">
         <v>57</v>
       </c>
@@ -2478,7 +2425,7 @@
       </c>
       <c r="G18" s="25"/>
     </row>
-    <row r="19" spans="1:7" ht="150">
+    <row r="19" spans="1:7" ht="150" x14ac:dyDescent="0.25">
       <c r="A19" s="24" t="s">
         <v>58</v>
       </c>
@@ -2495,7 +2442,7 @@
       </c>
       <c r="G19" s="25"/>
     </row>
-    <row r="20" spans="1:7" ht="135">
+    <row r="20" spans="1:7" ht="135" x14ac:dyDescent="0.25">
       <c r="A20" s="24" t="s">
         <v>59</v>
       </c>
@@ -2512,7 +2459,7 @@
       </c>
       <c r="G20" s="25"/>
     </row>
-    <row r="21" spans="1:7" ht="120">
+    <row r="21" spans="1:7" ht="120" x14ac:dyDescent="0.25">
       <c r="A21" s="24" t="s">
         <v>60</v>
       </c>
@@ -2529,7 +2476,7 @@
       </c>
       <c r="G21" s="25"/>
     </row>
-    <row r="22" spans="1:7" ht="120">
+    <row r="22" spans="1:7" ht="120" x14ac:dyDescent="0.25">
       <c r="A22" s="24" t="s">
         <v>61</v>
       </c>
@@ -2546,7 +2493,7 @@
       </c>
       <c r="G22" s="25"/>
     </row>
-    <row r="23" spans="1:7" ht="165">
+    <row r="23" spans="1:7" ht="165" x14ac:dyDescent="0.25">
       <c r="A23" s="24" t="s">
         <v>62</v>
       </c>
@@ -2563,7 +2510,7 @@
       </c>
       <c r="G23" s="25"/>
     </row>
-    <row r="24" spans="1:7" ht="165">
+    <row r="24" spans="1:7" ht="165" x14ac:dyDescent="0.25">
       <c r="A24" s="24" t="s">
         <v>63</v>
       </c>
@@ -2580,7 +2527,7 @@
       </c>
       <c r="G24" s="25"/>
     </row>
-    <row r="25" spans="1:7" ht="135">
+    <row r="25" spans="1:7" ht="135" x14ac:dyDescent="0.25">
       <c r="A25" s="24" t="s">
         <v>64</v>
       </c>
@@ -2597,7 +2544,7 @@
       </c>
       <c r="G25" s="25"/>
     </row>
-    <row r="26" spans="1:7" ht="135">
+    <row r="26" spans="1:7" ht="135" x14ac:dyDescent="0.25">
       <c r="A26" s="24" t="s">
         <v>65</v>
       </c>
@@ -2614,7 +2561,7 @@
       </c>
       <c r="G26" s="25"/>
     </row>
-    <row r="27" spans="1:7" ht="30">
+    <row r="27" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A27" s="28">
         <v>5.3</v>
       </c>
@@ -2627,7 +2574,7 @@
       <c r="F27" s="8"/>
       <c r="G27" s="29"/>
     </row>
-    <row r="28" spans="1:7" ht="105">
+    <row r="28" spans="1:7" ht="105" x14ac:dyDescent="0.25">
       <c r="A28" s="24" t="s">
         <v>72</v>
       </c>
@@ -2644,7 +2591,7 @@
       </c>
       <c r="G28" s="25"/>
     </row>
-    <row r="29" spans="1:7" ht="45">
+    <row r="29" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A29" s="24" t="s">
         <v>73</v>
       </c>
@@ -2661,7 +2608,7 @@
       </c>
       <c r="G29" s="25"/>
     </row>
-    <row r="30" spans="1:7" ht="120">
+    <row r="30" spans="1:7" ht="120" x14ac:dyDescent="0.25">
       <c r="A30" s="24" t="s">
         <v>74</v>
       </c>
@@ -2678,7 +2625,7 @@
       </c>
       <c r="G30" s="25"/>
     </row>
-    <row r="31" spans="1:7" ht="105">
+    <row r="31" spans="1:7" ht="105" x14ac:dyDescent="0.25">
       <c r="A31" s="24" t="s">
         <v>75</v>
       </c>
@@ -2695,7 +2642,7 @@
       </c>
       <c r="G31" s="25"/>
     </row>
-    <row r="32" spans="1:7" ht="60">
+    <row r="32" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A32" s="24" t="s">
         <v>76</v>
       </c>
@@ -2712,7 +2659,7 @@
       </c>
       <c r="G32" s="25"/>
     </row>
-    <row r="33" spans="1:7" ht="60">
+    <row r="33" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A33" s="24" t="s">
         <v>77</v>
       </c>
@@ -2729,7 +2676,7 @@
       </c>
       <c r="G33" s="25"/>
     </row>
-    <row r="34" spans="1:7" ht="60">
+    <row r="34" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A34" s="24" t="s">
         <v>78</v>
       </c>
@@ -2748,7 +2695,7 @@
       </c>
       <c r="G34" s="25"/>
     </row>
-    <row r="35" spans="1:7" ht="45">
+    <row r="35" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A35" s="24" t="s">
         <v>79</v>
       </c>
@@ -2767,7 +2714,7 @@
       </c>
       <c r="G35" s="25"/>
     </row>
-    <row r="36" spans="1:7" ht="45">
+    <row r="36" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A36" s="28" t="s">
         <v>245</v>
       </c>
@@ -2780,7 +2727,7 @@
       <c r="F36" s="8"/>
       <c r="G36" s="29"/>
     </row>
-    <row r="37" spans="1:7" ht="60">
+    <row r="37" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A37" s="24" t="s">
         <v>206</v>
       </c>
@@ -2797,7 +2744,7 @@
       </c>
       <c r="G37" s="25"/>
     </row>
-    <row r="38" spans="1:7" ht="60">
+    <row r="38" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A38" s="24" t="s">
         <v>207</v>
       </c>
@@ -2814,7 +2761,7 @@
       </c>
       <c r="G38" s="25"/>
     </row>
-    <row r="39" spans="1:7" ht="75">
+    <row r="39" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="A39" s="24" t="s">
         <v>208</v>
       </c>
@@ -2831,7 +2778,7 @@
       </c>
       <c r="G39" s="25"/>
     </row>
-    <row r="40" spans="1:7" ht="60">
+    <row r="40" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A40" s="24" t="s">
         <v>209</v>
       </c>
@@ -2848,7 +2795,7 @@
       </c>
       <c r="G40" s="25"/>
     </row>
-    <row r="41" spans="1:7" ht="75">
+    <row r="41" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="A41" s="24" t="s">
         <v>210</v>
       </c>
@@ -2865,7 +2812,7 @@
       </c>
       <c r="G41" s="25"/>
     </row>
-    <row r="42" spans="1:7" ht="75">
+    <row r="42" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="A42" s="24" t="s">
         <v>211</v>
       </c>
@@ -2882,7 +2829,7 @@
       </c>
       <c r="G42" s="25"/>
     </row>
-    <row r="43" spans="1:7" ht="30">
+    <row r="43" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A43" s="24" t="s">
         <v>212</v>
       </c>
@@ -2899,7 +2846,7 @@
       </c>
       <c r="G43" s="25"/>
     </row>
-    <row r="44" spans="1:7" ht="75">
+    <row r="44" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="A44" s="24" t="s">
         <v>205</v>
       </c>
@@ -2916,7 +2863,7 @@
       </c>
       <c r="G44" s="25"/>
     </row>
-    <row r="45" spans="1:7" ht="60">
+    <row r="45" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A45" s="24" t="s">
         <v>213</v>
       </c>
@@ -2933,7 +2880,7 @@
       </c>
       <c r="G45" s="25"/>
     </row>
-    <row r="46" spans="1:7" ht="60">
+    <row r="46" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A46" s="24" t="s">
         <v>214</v>
       </c>
@@ -2950,7 +2897,7 @@
       </c>
       <c r="G46" s="25"/>
     </row>
-    <row r="47" spans="1:7" ht="45">
+    <row r="47" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A47" s="24" t="s">
         <v>215</v>
       </c>
@@ -2967,7 +2914,7 @@
       </c>
       <c r="G47" s="25"/>
     </row>
-    <row r="48" spans="1:7" ht="30">
+    <row r="48" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A48" s="30">
         <v>5.4</v>
       </c>
@@ -2980,7 +2927,7 @@
       <c r="F48" s="10"/>
       <c r="G48" s="31"/>
     </row>
-    <row r="49" spans="1:7" ht="75">
+    <row r="49" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="A49" s="32" t="s">
         <v>86</v>
       </c>
@@ -2997,7 +2944,7 @@
       </c>
       <c r="G49" s="25"/>
     </row>
-    <row r="50" spans="1:7" ht="75">
+    <row r="50" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="A50" s="32" t="s">
         <v>87</v>
       </c>
@@ -3014,7 +2961,7 @@
       </c>
       <c r="G50" s="25"/>
     </row>
-    <row r="51" spans="1:7" ht="90">
+    <row r="51" spans="1:7" ht="90" x14ac:dyDescent="0.25">
       <c r="A51" s="32" t="s">
         <v>88</v>
       </c>
@@ -3031,7 +2978,7 @@
       </c>
       <c r="G51" s="25"/>
     </row>
-    <row r="52" spans="1:7" ht="75">
+    <row r="52" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="A52" s="32" t="s">
         <v>89</v>
       </c>
@@ -3048,7 +2995,7 @@
       </c>
       <c r="G52" s="25"/>
     </row>
-    <row r="53" spans="1:7" ht="75">
+    <row r="53" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="A53" s="32" t="s">
         <v>90</v>
       </c>
@@ -3065,7 +3012,7 @@
       </c>
       <c r="G53" s="25"/>
     </row>
-    <row r="54" spans="1:7" ht="75">
+    <row r="54" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="A54" s="32" t="s">
         <v>91</v>
       </c>
@@ -3082,7 +3029,7 @@
       </c>
       <c r="G54" s="25"/>
     </row>
-    <row r="55" spans="1:7" ht="150">
+    <row r="55" spans="1:7" ht="150" x14ac:dyDescent="0.25">
       <c r="A55" s="32" t="s">
         <v>92</v>
       </c>
@@ -3099,7 +3046,7 @@
       </c>
       <c r="G55" s="25"/>
     </row>
-    <row r="56" spans="1:7" ht="30">
+    <row r="56" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A56" s="30">
         <v>5.5</v>
       </c>
@@ -3112,7 +3059,7 @@
       <c r="F56" s="10"/>
       <c r="G56" s="31"/>
     </row>
-    <row r="57" spans="1:7" ht="75">
+    <row r="57" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="A57" s="32" t="s">
         <v>99</v>
       </c>
@@ -3129,7 +3076,7 @@
       </c>
       <c r="G57" s="25"/>
     </row>
-    <row r="58" spans="1:7" ht="60">
+    <row r="58" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A58" s="32" t="s">
         <v>100</v>
       </c>
@@ -3146,7 +3093,7 @@
       </c>
       <c r="G58" s="25"/>
     </row>
-    <row r="59" spans="1:7" ht="75">
+    <row r="59" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="A59" s="32" t="s">
         <v>101</v>
       </c>
@@ -3163,7 +3110,7 @@
       </c>
       <c r="G59" s="25"/>
     </row>
-    <row r="60" spans="1:7" ht="150">
+    <row r="60" spans="1:7" ht="150" x14ac:dyDescent="0.25">
       <c r="A60" s="32" t="s">
         <v>102</v>
       </c>
@@ -3180,7 +3127,7 @@
       </c>
       <c r="G60" s="25"/>
     </row>
-    <row r="61" spans="1:7" ht="45">
+    <row r="61" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A61" s="32" t="s">
         <v>103</v>
       </c>
@@ -3197,7 +3144,7 @@
       </c>
       <c r="G61" s="25"/>
     </row>
-    <row r="62" spans="1:7" ht="30">
+    <row r="62" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A62" s="40" t="s">
         <v>246</v>
       </c>
@@ -3210,7 +3157,7 @@
       <c r="F62" s="16"/>
       <c r="G62" s="34"/>
     </row>
-    <row r="63" spans="1:7" ht="30">
+    <row r="63" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A63" s="32" t="s">
         <v>116</v>
       </c>
@@ -3227,7 +3174,7 @@
       </c>
       <c r="G63" s="25"/>
     </row>
-    <row r="64" spans="1:7" ht="135">
+    <row r="64" spans="1:7" ht="135" x14ac:dyDescent="0.25">
       <c r="A64" s="32" t="s">
         <v>117</v>
       </c>
@@ -3244,7 +3191,7 @@
       </c>
       <c r="G64" s="25"/>
     </row>
-    <row r="65" spans="1:7" ht="60">
+    <row r="65" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A65" s="32" t="s">
         <v>118</v>
       </c>
@@ -3261,7 +3208,7 @@
       </c>
       <c r="G65" s="25"/>
     </row>
-    <row r="66" spans="1:7" ht="195">
+    <row r="66" spans="1:7" ht="195" x14ac:dyDescent="0.25">
       <c r="A66" s="32" t="s">
         <v>119</v>
       </c>
@@ -3278,7 +3225,7 @@
       </c>
       <c r="G66" s="25"/>
     </row>
-    <row r="67" spans="1:7" ht="75">
+    <row r="67" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="A67" s="32" t="s">
         <v>120</v>
       </c>
@@ -3295,7 +3242,7 @@
       </c>
       <c r="G67" s="25"/>
     </row>
-    <row r="68" spans="1:7" ht="150">
+    <row r="68" spans="1:7" ht="150" x14ac:dyDescent="0.25">
       <c r="A68" s="32" t="s">
         <v>121</v>
       </c>
@@ -3312,7 +3259,7 @@
       </c>
       <c r="G68" s="25"/>
     </row>
-    <row r="69" spans="1:7" ht="30">
+    <row r="69" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A69" s="40" t="s">
         <v>247</v>
       </c>
@@ -3325,7 +3272,7 @@
       <c r="F69" s="16"/>
       <c r="G69" s="34"/>
     </row>
-    <row r="70" spans="1:7" ht="60">
+    <row r="70" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A70" s="32" t="s">
         <v>122</v>
       </c>
@@ -3342,7 +3289,7 @@
       </c>
       <c r="G70" s="25"/>
     </row>
-    <row r="71" spans="1:7" ht="150">
+    <row r="71" spans="1:7" ht="150" x14ac:dyDescent="0.25">
       <c r="A71" s="32" t="s">
         <v>123</v>
       </c>
@@ -3359,7 +3306,7 @@
       </c>
       <c r="G71" s="25"/>
     </row>
-    <row r="72" spans="1:7" ht="60">
+    <row r="72" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A72" s="32" t="s">
         <v>124</v>
       </c>
@@ -3376,7 +3323,7 @@
       </c>
       <c r="G72" s="25"/>
     </row>
-    <row r="73" spans="1:7" ht="45">
+    <row r="73" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A73" s="40" t="s">
         <v>248</v>
       </c>
@@ -3389,7 +3336,7 @@
       <c r="F73" s="16"/>
       <c r="G73" s="34"/>
     </row>
-    <row r="74" spans="1:7" ht="105">
+    <row r="74" spans="1:7" ht="105" x14ac:dyDescent="0.25">
       <c r="A74" s="24" t="s">
         <v>126</v>
       </c>
@@ -3406,7 +3353,7 @@
       </c>
       <c r="G74" s="25"/>
     </row>
-    <row r="75" spans="1:7" ht="135">
+    <row r="75" spans="1:7" ht="135" x14ac:dyDescent="0.25">
       <c r="A75" s="24" t="s">
         <v>127</v>
       </c>
@@ -3423,7 +3370,7 @@
       </c>
       <c r="G75" s="25"/>
     </row>
-    <row r="76" spans="1:7" ht="165">
+    <row r="76" spans="1:7" ht="165" x14ac:dyDescent="0.25">
       <c r="A76" s="24" t="s">
         <v>128</v>
       </c>
@@ -3440,7 +3387,7 @@
       </c>
       <c r="G76" s="25"/>
     </row>
-    <row r="77" spans="1:7" ht="165">
+    <row r="77" spans="1:7" ht="165" x14ac:dyDescent="0.25">
       <c r="A77" s="24" t="s">
         <v>129</v>
       </c>
@@ -3457,7 +3404,7 @@
       </c>
       <c r="G77" s="25"/>
     </row>
-    <row r="78" spans="1:7" ht="150">
+    <row r="78" spans="1:7" ht="150" x14ac:dyDescent="0.25">
       <c r="A78" s="24" t="s">
         <v>130</v>
       </c>
@@ -3474,7 +3421,7 @@
       </c>
       <c r="G78" s="25"/>
     </row>
-    <row r="79" spans="1:7" ht="135">
+    <row r="79" spans="1:7" ht="135" x14ac:dyDescent="0.25">
       <c r="A79" s="24" t="s">
         <v>131</v>
       </c>
@@ -3491,7 +3438,7 @@
       </c>
       <c r="G79" s="25"/>
     </row>
-    <row r="80" spans="1:7" ht="180">
+    <row r="80" spans="1:7" ht="180" x14ac:dyDescent="0.25">
       <c r="A80" s="24" t="s">
         <v>132</v>
       </c>
@@ -3508,7 +3455,7 @@
       </c>
       <c r="G80" s="25"/>
     </row>
-    <row r="81" spans="1:7" ht="165">
+    <row r="81" spans="1:7" ht="165" x14ac:dyDescent="0.25">
       <c r="A81" s="24" t="s">
         <v>133</v>
       </c>
@@ -3525,7 +3472,7 @@
       </c>
       <c r="G81" s="25"/>
     </row>
-    <row r="82" spans="1:7" ht="135">
+    <row r="82" spans="1:7" ht="135" x14ac:dyDescent="0.25">
       <c r="A82" s="24" t="s">
         <v>134</v>
       </c>
@@ -3542,7 +3489,7 @@
       </c>
       <c r="G82" s="25"/>
     </row>
-    <row r="83" spans="1:7" ht="150">
+    <row r="83" spans="1:7" ht="150" x14ac:dyDescent="0.25">
       <c r="A83" s="24" t="s">
         <v>135</v>
       </c>
@@ -3559,7 +3506,7 @@
       </c>
       <c r="G83" s="25"/>
     </row>
-    <row r="84" spans="1:7" ht="45">
+    <row r="84" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A84" s="40" t="s">
         <v>249</v>
       </c>
@@ -3572,7 +3519,7 @@
       <c r="F84" s="16"/>
       <c r="G84" s="34"/>
     </row>
-    <row r="85" spans="1:7" ht="165">
+    <row r="85" spans="1:7" ht="165" x14ac:dyDescent="0.25">
       <c r="A85" s="24" t="s">
         <v>138</v>
       </c>
@@ -3589,7 +3536,7 @@
       </c>
       <c r="G85" s="25"/>
     </row>
-    <row r="86" spans="1:7" ht="90">
+    <row r="86" spans="1:7" ht="90" x14ac:dyDescent="0.25">
       <c r="A86" s="24" t="s">
         <v>139</v>
       </c>
@@ -3606,7 +3553,7 @@
       </c>
       <c r="G86" s="25"/>
     </row>
-    <row r="87" spans="1:7" ht="195">
+    <row r="87" spans="1:7" ht="195" x14ac:dyDescent="0.25">
       <c r="A87" s="24" t="s">
         <v>140</v>
       </c>
@@ -3623,7 +3570,7 @@
       </c>
       <c r="G87" s="25"/>
     </row>
-    <row r="88" spans="1:7" ht="180">
+    <row r="88" spans="1:7" ht="180" x14ac:dyDescent="0.25">
       <c r="A88" s="24" t="s">
         <v>241</v>
       </c>
@@ -3640,7 +3587,7 @@
       </c>
       <c r="G88" s="25"/>
     </row>
-    <row r="89" spans="1:7" ht="30">
+    <row r="89" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A89" s="24" t="s">
         <v>242</v>
       </c>
@@ -3657,7 +3604,7 @@
       </c>
       <c r="G89" s="25"/>
     </row>
-    <row r="90" spans="1:7" ht="60.75" thickBot="1">
+    <row r="90" spans="1:7" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A90" s="35" t="s">
         <v>243</v>
       </c>
@@ -3674,22 +3621,22 @@
       </c>
       <c r="G90" s="39"/>
     </row>
-    <row r="306" spans="1:1">
+    <row r="306" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A306" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="307" spans="1:1">
+    <row r="307" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A307" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="308" spans="1:1">
+    <row r="308" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A308" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="309" spans="1:1">
+    <row r="309" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A309" t="s">
         <v>8</v>
       </c>
@@ -3708,13 +3655,13 @@
     <mergeCell ref="M3:M4"/>
   </mergeCells>
   <conditionalFormatting sqref="F57:F61 F74:F83 F70:F72 F63:F68 F49:F55 F7:F11 F17:F26 F13:F15 F28:F35 F85:F90 F37:F47">
-    <cfRule type="containsText" dxfId="8" priority="31" operator="containsText" text="BLOCKED">
+    <cfRule type="containsText" dxfId="2" priority="31" operator="containsText" text="BLOCKED">
       <formula>NOT(ISERROR(SEARCH("BLOCKED",F7)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="7" priority="32" operator="containsText" text="FAIL">
+    <cfRule type="containsText" dxfId="1" priority="32" operator="containsText" text="FAIL">
       <formula>NOT(ISERROR(SEARCH("FAIL",F7)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="6" priority="33" operator="containsText" text="PASS">
+    <cfRule type="containsText" dxfId="0" priority="33" operator="containsText" text="PASS">
       <formula>NOT(ISERROR(SEARCH("PASS",F7)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -3729,39 +3676,39 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E17"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D21" sqref="D21"/>
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:5">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:5">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:5">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>147</v>
       </c>
@@ -3778,7 +3725,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="1:5">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="48">
         <v>6</v>
       </c>
@@ -3799,7 +3746,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:5">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="48">
         <v>6.1</v>
       </c>
@@ -3820,7 +3767,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:5">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="48">
         <v>6.2</v>
       </c>
@@ -3841,7 +3788,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:5">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="48">
         <v>6.3</v>
       </c>
@@ -3862,150 +3809,169 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:5">
-      <c r="A11" s="48">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" s="48"/>
+      <c r="B11" s="49">
+        <f>COUNTIF(Sheet1!F37:F47, Sheet2!B6)</f>
+        <v>0</v>
+      </c>
+      <c r="C11" s="49">
+        <f>COUNTIF(Sheet1!F37:F47, Sheet2!C6)</f>
+        <v>0</v>
+      </c>
+      <c r="D11" s="49">
+        <f>COUNTIF(Sheet1!F37:F47, Sheet2!D6)</f>
+        <v>11</v>
+      </c>
+      <c r="E11" s="49">
+        <f>COUNTIF(Sheet1!F37:F47, Sheet2!E6)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" s="48">
         <v>6.4</v>
       </c>
-      <c r="B11" s="49">
+      <c r="B12" s="49">
         <f>COUNTIF(Sheet1!F49:F55, Sheet2!B6)</f>
         <v>0</v>
       </c>
-      <c r="C11" s="49">
+      <c r="C12" s="49">
         <f>COUNTIF(Sheet1!F49:F55, Sheet2!C6)</f>
         <v>0</v>
       </c>
-      <c r="D11" s="49">
+      <c r="D12" s="49">
         <f>COUNTIF(Sheet1!F49:F55, Sheet2!D6)</f>
         <v>7</v>
       </c>
-      <c r="E11" s="49">
+      <c r="E12" s="49">
         <f>COUNTIF(Sheet1!F49:F55, Sheet2!E6)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:5">
-      <c r="A12" s="48">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" s="48">
         <v>6.5</v>
       </c>
-      <c r="B12" s="49">
+      <c r="B13" s="49">
         <f>COUNTIF(Sheet1!F57:F61, Sheet2!B6)</f>
         <v>0</v>
       </c>
-      <c r="C12" s="49">
+      <c r="C13" s="49">
         <f>COUNTIF(Sheet1!F57:F61, Sheet2!C6)</f>
         <v>0</v>
       </c>
-      <c r="D12" s="49">
+      <c r="D13" s="49">
         <f>COUNTIF(Sheet1!F57:F61, Sheet2!D6)</f>
         <v>5</v>
       </c>
-      <c r="E12" s="49">
+      <c r="E13" s="49">
         <f>COUNTIF(Sheet1!F57:F61, Sheet2!E6)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:5">
-      <c r="A13" s="48" t="s">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" s="48" t="s">
         <v>105</v>
       </c>
-      <c r="B13" s="49">
+      <c r="B14" s="49">
         <f>COUNTIF(Sheet1!F63:F68, Sheet2!B6)</f>
         <v>0</v>
       </c>
-      <c r="C13" s="49">
+      <c r="C14" s="49">
         <f>COUNTIF(Sheet1!F63:F68, Sheet2!C6)</f>
         <v>0</v>
       </c>
-      <c r="D13" s="49">
+      <c r="D14" s="49">
         <f>COUNTIF(Sheet1!F63:F68, Sheet2!D6)</f>
         <v>6</v>
       </c>
-      <c r="E13" s="49">
+      <c r="E14" s="49">
         <f>COUNTIF(Sheet1!F63:F68, Sheet2!E6)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:5">
-      <c r="A14" s="48" t="s">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" s="48" t="s">
         <v>111</v>
       </c>
-      <c r="B14" s="49">
+      <c r="B15" s="49">
         <f>COUNTIF(Sheet1!F70:F72, Sheet2!B6)</f>
         <v>0</v>
       </c>
-      <c r="C14" s="49">
+      <c r="C15" s="49">
         <f>COUNTIF(Sheet1!F70:F72, Sheet2!C6)</f>
         <v>0</v>
       </c>
-      <c r="D14" s="49">
+      <c r="D15" s="49">
         <f>COUNTIF(Sheet1!F70:F72, Sheet2!D6)</f>
         <v>3</v>
       </c>
-      <c r="E14" s="49">
+      <c r="E15" s="49">
         <f>COUNTIF(Sheet1!F70:F72, Sheet2!E6)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:5">
-      <c r="A15" s="48" t="s">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" s="48" t="s">
         <v>115</v>
       </c>
-      <c r="B15" s="49">
+      <c r="B16" s="49">
         <f>COUNTIF(Sheet1!F74:F83, Sheet2!B6)</f>
         <v>0</v>
       </c>
-      <c r="C15" s="49">
+      <c r="C16" s="49">
         <f>COUNTIF(Sheet1!F74:F83, Sheet2!C6)</f>
         <v>0</v>
       </c>
-      <c r="D15" s="49">
+      <c r="D16" s="49">
         <f>COUNTIF(Sheet1!F74:F83, Sheet2!D6)</f>
         <v>10</v>
       </c>
-      <c r="E15" s="49">
+      <c r="E16" s="49">
         <f>COUNTIF(Sheet1!F74:F83, Sheet2!E6)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:5">
-      <c r="A16" s="48" t="s">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" s="48" t="s">
         <v>141</v>
       </c>
-      <c r="B16" s="49">
+      <c r="B17" s="49">
         <f>COUNTIF(Sheet1!F85:F90, Sheet2!B6)</f>
         <v>0</v>
       </c>
-      <c r="C16" s="49">
+      <c r="C17" s="49">
         <f>COUNTIF(Sheet1!F85:F90, Sheet2!C6)</f>
         <v>0</v>
       </c>
-      <c r="D16" s="49">
+      <c r="D17" s="49">
         <f>COUNTIF(Sheet1!F85:F90, Sheet2!D6)</f>
         <v>6</v>
       </c>
-      <c r="E16" s="49">
+      <c r="E17" s="49">
         <f>COUNTIF(Sheet1!F85:F90, Sheet2!E6)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:5">
-      <c r="A17" s="48" t="s">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" s="48" t="s">
         <v>148</v>
       </c>
-      <c r="B17">
-        <f>SUM(B7:B16)</f>
+      <c r="B18">
+        <f>SUM(B7:B17)</f>
         <v>0</v>
       </c>
-      <c r="C17">
-        <f>SUM(C7:C16)</f>
+      <c r="C18">
+        <f>SUM(C7:C17)</f>
         <v>0</v>
       </c>
-      <c r="D17">
-        <f>SUM(D7:D16)</f>
-        <v>63</v>
-      </c>
-      <c r="E17">
-        <f>SUM(E7:E16)</f>
+      <c r="D18">
+        <f>SUM(D7:D17)</f>
+        <v>74</v>
+      </c>
+      <c r="E18">
+        <f>SUM(E7:E17)</f>
         <v>0</v>
       </c>
     </row>
@@ -4015,31 +3981,31 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:1">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:1">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:1">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:1">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>8</v>
       </c>

</xml_diff>